<commit_message>
Added custom mapping specifications
</commit_message>
<xml_diff>
--- a/Custom Mapping Specifications.xlsx
+++ b/Custom Mapping Specifications.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Business\GitHub\sfec_to_wfs_cpi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A24269-0EA3-485E-9841-7C3678FE1C6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4AB9B3-2913-46B1-8E2A-5BF1C6D15614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1C4D54CC-346F-4E9A-B38A-1F60A76234FC}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{1C4D54CC-346F-4E9A-B38A-1F60A76234FC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -888,16 +888,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C2C045-56B9-490E-8185-F4BBA8ED695D}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="31" style="1" customWidth="1"/>
-    <col min="3" max="3" width="50.36328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="29.81640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.1796875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="80.90625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" style="1"/>
   </cols>

</xml_diff>